<commit_message>
Fix the bugs in the last merge
</commit_message>
<xml_diff>
--- a/src/DIVA_maces.xlsx
+++ b/src/DIVA_maces.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanz151/Python_maces/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB89C2A-6F8B-BA48-899B-EA68AD9FFD6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9E1049-0F9D-184C-8477-5363205EB561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16520" xr2:uid="{0E9594E8-19DA-F347-AAA7-44D762B0FCB8}"/>
+    <workbookView xWindow="14120" yWindow="2240" windowWidth="28800" windowHeight="16520" xr2:uid="{0E9594E8-19DA-F347-AAA7-44D762B0FCB8}"/>
   </bookViews>
   <sheets>
     <sheet name="diva" sheetId="1" r:id="rId1"/>
@@ -546,11 +546,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404D9C3E-F266-A845-AF6C-B416CDC68752}">
-  <dimension ref="A1:AU2"/>
+  <dimension ref="A1:AU4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,7 +722,7 @@
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>466</v>
       </c>
       <c r="B2" s="5">
         <v>45.555999999999997</v>
@@ -860,6 +860,292 @@
         <v>-1</v>
       </c>
       <c r="AU2" s="5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>466</v>
+      </c>
+      <c r="B3" s="5">
+        <v>45.555999999999997</v>
+      </c>
+      <c r="C3" s="5">
+        <v>12.458</v>
+      </c>
+      <c r="D3" s="5">
+        <v>113.059584</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.84166300000000005</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.58103300000000002</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.24166000000000001</v>
+      </c>
+      <c r="H3" s="5">
+        <v>6.4243999999999996E-2</v>
+      </c>
+      <c r="I3" s="5">
+        <v>9.4105699999999999</v>
+      </c>
+      <c r="J3" s="5">
+        <v>28</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>339.17952000000002</v>
+      </c>
+      <c r="O3" s="5">
+        <v>621.82771200000002</v>
+      </c>
+      <c r="P3" s="5">
+        <v>508.76812799999999</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>418.32046079999998</v>
+      </c>
+      <c r="R3" s="5">
+        <v>192.2012928</v>
+      </c>
+      <c r="S3" s="5">
+        <v>768.80517120000002</v>
+      </c>
+      <c r="T3" s="5">
+        <v>1175.8196736</v>
+      </c>
+      <c r="U3" s="5">
+        <v>0</v>
+      </c>
+      <c r="V3" s="5">
+        <v>0</v>
+      </c>
+      <c r="W3" s="5">
+        <v>0</v>
+      </c>
+      <c r="X3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>15.6</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="AD3">
+        <v>1.6</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="5">
+        <v>2</v>
+      </c>
+      <c r="AM3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AQ3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AR3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AS3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AU3" s="5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>466</v>
+      </c>
+      <c r="B4" s="5">
+        <v>45.555999999999997</v>
+      </c>
+      <c r="C4" s="5">
+        <v>12.458</v>
+      </c>
+      <c r="D4" s="5">
+        <v>113.059584</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.84166300000000005</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.58103300000000002</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.24166000000000001</v>
+      </c>
+      <c r="H4" s="5">
+        <v>6.4243999999999996E-2</v>
+      </c>
+      <c r="I4" s="5">
+        <v>9.4105699999999999</v>
+      </c>
+      <c r="J4" s="5">
+        <v>28</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>339.17952000000002</v>
+      </c>
+      <c r="O4" s="5">
+        <v>621.82771200000002</v>
+      </c>
+      <c r="P4" s="5">
+        <v>508.76812799999999</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>418.32046079999998</v>
+      </c>
+      <c r="R4" s="5">
+        <v>192.2012928</v>
+      </c>
+      <c r="S4" s="5">
+        <v>768.80517120000002</v>
+      </c>
+      <c r="T4" s="5">
+        <v>1175.8196736</v>
+      </c>
+      <c r="U4" s="5">
+        <v>0</v>
+      </c>
+      <c r="V4" s="5">
+        <v>0</v>
+      </c>
+      <c r="W4" s="5">
+        <v>0</v>
+      </c>
+      <c r="X4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>15.6</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="AD4">
+        <v>1.6</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="5">
+        <v>2</v>
+      </c>
+      <c r="AM4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AP4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AQ4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AR4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AS4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AT4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AU4" s="5">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test steady-state wave dynamics
</commit_message>
<xml_diff>
--- a/src/DIVA_maces.xlsx
+++ b/src/DIVA_maces.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanz151/Python_maces/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9E1049-0F9D-184C-8477-5363205EB561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBC7B0B-657A-0C43-AB13-8A490DAFA56F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14120" yWindow="2240" windowWidth="28800" windowHeight="16520" xr2:uid="{0E9594E8-19DA-F347-AAA7-44D762B0FCB8}"/>
+    <workbookView xWindow="8640" yWindow="5500" windowWidth="28800" windowHeight="16520" xr2:uid="{0E9594E8-19DA-F347-AAA7-44D762B0FCB8}"/>
   </bookViews>
   <sheets>
     <sheet name="diva" sheetId="1" r:id="rId1"/>
@@ -865,7 +865,7 @@
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B3" s="5">
         <v>45.555999999999997</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B4" s="5">
         <v>45.555999999999997</v>

</xml_diff>